<commit_message>
updated area table to include parking information.
Also, included new table for parking information.
</commit_message>
<xml_diff>
--- a/Areas.xlsx
+++ b/Areas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jmill/Documents/Projects/BasicConnection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{827F8D0A-097D-8F43-BFC4-F35091A38A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D097273D-B387-3A4E-8A66-8F273EEBE7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F9CA1732-CA54-B647-AFB8-F45285882BC5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{F9CA1732-CA54-B647-AFB8-F45285882BC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="46">
   <si>
     <t>destination</t>
   </si>
@@ -55,12 +55,6 @@
     <t>sun</t>
   </si>
   <si>
-    <t>parking_lat</t>
-  </si>
-  <si>
-    <t>parking_long</t>
-  </si>
-  <si>
     <t>rain_covered</t>
   </si>
   <si>
@@ -164,6 +158,21 @@
   </si>
   <si>
     <t>Parking Lot</t>
+  </si>
+  <si>
+    <t>parking</t>
+  </si>
+  <si>
+    <t>Day-use Parking South</t>
+  </si>
+  <si>
+    <t>Day-use Parking North</t>
+  </si>
+  <si>
+    <t>Viewpoint Parking</t>
+  </si>
+  <si>
+    <t>Apron Parking</t>
   </si>
 </sst>
 </file>
@@ -515,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1A66BF0-B191-8C4D-996A-C3F14488B890}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,12 +538,12 @@
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -557,890 +566,812 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
       <c r="D2">
         <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="H2">
-        <v>49.679079999999999</v>
-      </c>
-      <c r="I2">
-        <v>-123.15461999999999</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
       <c r="D3">
         <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3">
-        <v>49.680639999999997</v>
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
       </c>
       <c r="I3">
-        <v>-123.15324</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4">
-        <v>49.680639999999997</v>
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
       </c>
       <c r="I4">
-        <v>-123.15324</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <v>49.680639999999997</v>
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
       </c>
       <c r="I5">
-        <v>-123.15324</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6">
-        <v>49.680639999999997</v>
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
       </c>
       <c r="I6">
-        <v>-123.15324</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
       </c>
       <c r="I7">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F8">
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
       </c>
       <c r="I8">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F9">
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
       </c>
       <c r="I9">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10">
         <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F10">
         <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
       </c>
       <c r="I10">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11">
         <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F11">
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
       </c>
       <c r="I11">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>119</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F12">
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
       </c>
       <c r="I12">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13">
         <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
       </c>
       <c r="I13">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14">
         <v>94</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F14">
         <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>44</v>
       </c>
       <c r="I14">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15">
         <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F15">
         <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
       </c>
       <c r="I15">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F16">
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>44</v>
       </c>
       <c r="I16">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17">
         <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F17">
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
       </c>
       <c r="I17">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F18">
         <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>44</v>
       </c>
       <c r="I18">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19">
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F19">
         <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>44</v>
       </c>
       <c r="I19">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20">
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F20">
         <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20">
-        <v>49.681870000000004</v>
+        <v>12</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
       </c>
       <c r="I20">
-        <v>-123.15331</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21">
         <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F21">
         <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21">
-        <v>49.681899999999999</v>
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
+        <v>44</v>
       </c>
       <c r="I21">
-        <v>-123.1533</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D22">
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F22">
         <v>8</v>
       </c>
       <c r="G22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
         <v>37</v>
-      </c>
-      <c r="H22">
-        <v>49.681899999999999</v>
-      </c>
-      <c r="I22">
-        <v>-123.1533</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" t="s">
-        <v>39</v>
       </c>
       <c r="D23">
         <v>86</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F23">
         <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23">
-        <v>49.681899999999999</v>
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>44</v>
       </c>
       <c r="I23">
-        <v>-123.1533</v>
+        <v>1</v>
       </c>
       <c r="J23">
         <v>1</v>
       </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F24">
         <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24">
-        <v>49.681899999999999</v>
+        <v>35</v>
+      </c>
+      <c r="H24" t="s">
+        <v>44</v>
       </c>
       <c r="I24">
-        <v>-123.1533</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D25">
         <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F25">
         <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25">
-        <v>49.688299999999998</v>
+        <v>35</v>
+      </c>
+      <c r="H25" t="s">
+        <v>45</v>
       </c>
       <c r="I25">
-        <v>-123.1472</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D26">
         <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F26">
         <v>5</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26">
-        <v>49.688299999999998</v>
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>45</v>
       </c>
       <c r="I26">
-        <v>-123.1472</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
         <v>0</v>
       </c>
     </row>

</xml_diff>